<commit_message>
footer e nav php componentes
</commit_message>
<xml_diff>
--- a/Arquivos/cronograma_tcc.xlsx
+++ b/Arquivos/cronograma_tcc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\TCC\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBB784A-5FCA-4015-ACAF-01D660ABEA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E2AFB2-0183-4FC2-85B7-713792DDB8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BBDFA246-CB9F-4529-AFA9-E3C590C6F618}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="83">
   <si>
     <t>Designer</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Footer</t>
   </si>
   <si>
-    <t>Código</t>
-  </si>
-  <si>
     <t>HTML e CSS base - Home</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Wireframe - Área administrativa CRUD animais</t>
   </si>
   <si>
-    <t>HTML e CSS base - Doações e Animais</t>
-  </si>
-  <si>
     <t>Informação dos animais</t>
   </si>
   <si>
@@ -228,9 +222,6 @@
     <t>CSS - Home</t>
   </si>
   <si>
-    <t>Folha de rosto e Dados de instalação</t>
-  </si>
-  <si>
     <t>CSS - Animais</t>
   </si>
   <si>
@@ -286,13 +277,25 @@
   </si>
   <si>
     <t>Adiado</t>
+  </si>
+  <si>
+    <t>Criação do banco e tabelas de animais, doações, adm e mensagens</t>
+  </si>
+  <si>
+    <t>Atualizações nas tabelas</t>
+  </si>
+  <si>
+    <t>HTML e CSS base - Criação pg de Doações e Animais</t>
+  </si>
+  <si>
+    <t>Folha de rosto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +312,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -573,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -678,12 +688,836 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="100">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6699FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6699FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -766,6 +1600,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF6699FF"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FFFFCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1220,7 +2062,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1230,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351F5228-FEA6-410A-9456-2C6350ABE72B}">
   <dimension ref="C2:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +2110,7 @@
         <v>17</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I2" s="41"/>
       <c r="J2" s="1" t="s">
@@ -1281,8 +2123,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="42" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -1311,8 +2153,8 @@
       </c>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="43" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="29" t="s">
@@ -1342,11 +2184,11 @@
       <c r="L4" s="36"/>
     </row>
     <row r="5" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="44" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="13">
         <v>45385</v>
@@ -1371,8 +2213,8 @@
       </c>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="29" t="s">
@@ -1401,8 +2243,8 @@
       </c>
       <c r="L6" s="36"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C7" s="44" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="27" t="s">
@@ -1431,8 +2273,8 @@
       </c>
       <c r="L7" s="38"/>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
+    <row r="8" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="43" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -1461,12 +2303,12 @@
       </c>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+    <row r="9" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="44" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E9" s="13">
         <v>45387</v>
@@ -1491,8 +2333,8 @@
       </c>
       <c r="L9" s="38"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="10" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="29" t="s">
@@ -1521,8 +2363,8 @@
       </c>
       <c r="L10" s="36"/>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="27" t="s">
@@ -1551,8 +2393,8 @@
       </c>
       <c r="L11" s="38"/>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="3" t="s">
+    <row r="12" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="29" t="s">
@@ -1581,8 +2423,8 @@
       </c>
       <c r="L12" s="36"/>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="44" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -1611,8 +2453,8 @@
       </c>
       <c r="L13" s="38"/>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
+    <row r="14" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="43" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="29" t="s">
@@ -1641,12 +2483,12 @@
       </c>
       <c r="L14" s="36"/>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="44" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="13">
         <v>45396</v>
@@ -1671,12 +2513,12 @@
       </c>
       <c r="L15" s="38"/>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
+    <row r="16" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="E16" s="12">
         <v>45397</v>
@@ -1701,12 +2543,12 @@
       </c>
       <c r="L16" s="36"/>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+    <row r="17" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="13">
         <v>45398</v>
@@ -1731,12 +2573,12 @@
       </c>
       <c r="L17" s="38"/>
     </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+    <row r="18" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C18" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E18" s="12">
         <v>45400</v>
@@ -1761,12 +2603,12 @@
       </c>
       <c r="L18" s="36"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="44" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="13">
         <v>45401</v>
@@ -1791,8 +2633,8 @@
       </c>
       <c r="L19" s="38"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
+    <row r="20" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C20" s="43" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="29" t="s">
@@ -1821,12 +2663,12 @@
       </c>
       <c r="L20" s="36"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
+    <row r="21" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="44" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="13">
         <v>45403</v>
@@ -1851,12 +2693,12 @@
       </c>
       <c r="L21" s="38"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+    <row r="22" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E22" s="12">
         <v>45404</v>
@@ -1882,12 +2724,12 @@
       <c r="L22" s="36"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="E23" s="13">
         <v>45405</v>
@@ -1913,12 +2755,12 @@
       <c r="L23" s="38"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
+    <row r="24" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C24" s="43" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E24" s="12">
         <v>45404</v>
@@ -1944,8 +2786,8 @@
       <c r="L24" s="36"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C25" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="27" t="s">
@@ -1975,12 +2817,12 @@
       <c r="L25" s="38"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C26" s="3" t="s">
+    <row r="26" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C26" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E26" s="12">
         <v>45408</v>
@@ -2006,12 +2848,12 @@
       <c r="L26" s="36"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C27" s="4" t="s">
+    <row r="27" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C27" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E27" s="13">
         <v>45409</v>
@@ -2038,11 +2880,11 @@
       <c r="P27" s="10"/>
     </row>
     <row r="28" spans="3:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="12">
         <v>45410</v>
@@ -2068,8 +2910,8 @@
       <c r="L28" s="36"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C29" s="4" t="s">
+    <row r="29" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="27" t="s">
@@ -2098,12 +2940,12 @@
       </c>
       <c r="L29" s="38"/>
     </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="3" t="s">
+    <row r="30" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C30" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30" s="12">
         <v>45411</v>
@@ -2127,15 +2969,15 @@
         <v>0</v>
       </c>
       <c r="L30" s="36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C31" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E31" s="13">
         <v>45412</v>
@@ -2160,12 +3002,12 @@
       </c>
       <c r="L31" s="38"/>
     </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
+    <row r="32" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C32" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E32" s="12">
         <v>45414</v>
@@ -2190,12 +3032,12 @@
       </c>
       <c r="L32" s="36"/>
     </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
+    <row r="33" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E33" s="13">
         <v>45415</v>
@@ -2220,12 +3062,12 @@
       </c>
       <c r="L33" s="38"/>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+    <row r="34" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C34" s="43" t="s">
         <v>30</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E34" s="12">
         <v>45416</v>
@@ -2250,8 +3092,8 @@
       </c>
       <c r="L34" s="36"/>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
+    <row r="35" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C35" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="27" t="s">
@@ -2280,12 +3122,12 @@
       </c>
       <c r="L35" s="38"/>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C36" s="3" t="s">
+    <row r="36" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C36" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E36" s="12">
         <v>45418</v>
@@ -2309,15 +3151,15 @@
         <v>0</v>
       </c>
       <c r="L36" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E37" s="13">
         <v>45419</v>
@@ -2342,12 +3184,12 @@
       </c>
       <c r="L37" s="38"/>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="3" t="s">
+    <row r="38" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C38" s="43" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E38" s="12">
         <v>45422</v>
@@ -2372,8 +3214,8 @@
       </c>
       <c r="L38" s="36"/>
     </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="4" t="s">
+    <row r="39" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="27" t="s">
@@ -2402,12 +3244,12 @@
       </c>
       <c r="L39" s="38"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C40" s="3" t="s">
+    <row r="40" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C40" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" s="12">
         <v>45425</v>
@@ -2431,15 +3273,15 @@
         <v>0</v>
       </c>
       <c r="L40" s="36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C41" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C41" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E41" s="13">
         <v>45427</v>
@@ -2457,19 +3299,19 @@
         <v>27</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K41" s="15">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L41" s="38"/>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
+    <row r="42" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C42" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E42" s="12">
         <v>45430</v>
@@ -2494,8 +3336,8 @@
       </c>
       <c r="L42" s="36"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C43" s="4" t="s">
+    <row r="43" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C43" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="27" t="s">
@@ -2524,12 +3366,12 @@
       </c>
       <c r="L43" s="38"/>
     </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C44" s="3" t="s">
+    <row r="44" spans="3:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="43" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E44" s="12">
         <v>45436</v>
@@ -2553,15 +3395,15 @@
         <v>0</v>
       </c>
       <c r="L44" s="36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="44" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E45" s="13">
         <v>45439</v>
@@ -2579,19 +3421,19 @@
         <v>27</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K45" s="15">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L45" s="38"/>
     </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C46" s="3" t="s">
+    <row r="46" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C46" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E46" s="12">
         <v>45442</v>
@@ -2612,12 +3454,12 @@
         <v>19</v>
       </c>
       <c r="K46" s="15">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="L46" s="36"/>
     </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
+    <row r="47" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C47" s="44" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="27" t="s">
@@ -2646,12 +3488,12 @@
       </c>
       <c r="L47" s="38"/>
     </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C48" s="3" t="s">
+    <row r="48" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C48" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="E48" s="12">
         <v>45439</v>
@@ -2669,19 +3511,19 @@
         <v>6</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K48" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L48" s="36"/>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C49" s="4" t="s">
+    <row r="49" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C49" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E49" s="13">
         <v>45446</v>
@@ -2706,12 +3548,12 @@
       </c>
       <c r="L49" s="38"/>
     </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C50" s="3" t="s">
+    <row r="50" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C50" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E50" s="12">
         <v>45451</v>
@@ -2736,12 +3578,12 @@
       </c>
       <c r="L50" s="36"/>
     </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="4" t="s">
+    <row r="51" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C51" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E51" s="13">
         <v>45454</v>
@@ -2766,12 +3608,12 @@
       </c>
       <c r="L51" s="38"/>
     </row>
-    <row r="52" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C52" s="3" t="s">
+    <row r="52" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C52" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E52" s="12">
         <v>45458</v>
@@ -2796,12 +3638,12 @@
       </c>
       <c r="L52" s="36"/>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="4" t="s">
+    <row r="53" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C53" s="44" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E53" s="13">
         <v>45467</v>
@@ -2826,12 +3668,12 @@
       </c>
       <c r="L53" s="38"/>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
+    <row r="54" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C54" s="43" t="s">
         <v>1</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E54" s="12">
         <v>45471</v>
@@ -2856,12 +3698,12 @@
       </c>
       <c r="L54" s="36"/>
     </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C55" s="4" t="s">
+    <row r="55" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C55" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E55" s="13">
         <v>45443</v>
@@ -2886,12 +3728,12 @@
       </c>
       <c r="L55" s="38"/>
     </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
+    <row r="56" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C56" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E56" s="12">
         <v>45450</v>
@@ -2916,12 +3758,12 @@
       </c>
       <c r="L56" s="36"/>
     </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C57" s="4" t="s">
+    <row r="57" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C57" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E57" s="13">
         <v>45453</v>
@@ -2946,12 +3788,12 @@
       </c>
       <c r="L57" s="38"/>
     </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
+    <row r="58" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C58" s="43" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E58" s="12">
         <v>45457</v>
@@ -2976,12 +3818,12 @@
       </c>
       <c r="L58" s="36"/>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C59" s="4" t="s">
+    <row r="59" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C59" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E59" s="13">
         <v>45460</v>
@@ -3006,12 +3848,12 @@
       </c>
       <c r="L59" s="38"/>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C60" s="30" t="s">
+    <row r="60" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C60" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E60" s="32">
         <v>45575</v>
@@ -3038,17 +3880,17 @@
     </row>
     <row r="62" spans="3:12" ht="60" x14ac:dyDescent="0.25">
       <c r="C62" s="35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="3:12" ht="30" x14ac:dyDescent="0.25">
       <c r="C63" s="35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C64" s="35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3057,28 +3899,54 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A12:A15">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J60">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Finalizado">
+    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Finalizado">
       <formula>NOT(ISERROR(SEARCH("Finalizado",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="A fazer">
+    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="A fazer">
       <formula>NOT(ISERROR(SEARCH("A fazer",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Em progresso">
+    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Em progresso">
       <formula>NOT(ISERROR(SEARCH("Em progresso",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K60">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C60">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="Front-End">
+      <formula>NOT(ISERROR(SEARCH("Front-End",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Back-End">
+      <formula>NOT(ISERROR(SEARCH("Back-End",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Design">
+      <formula>NOT(ISERROR(SEARCH("Design",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Planejamento">
+      <formula>NOT(ISERROR(SEARCH("Planejamento",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Conteúdo">
+      <formula>NOT(ISERROR(SEARCH("Conteúdo",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Documentação">
+      <formula>NOT(ISERROR(SEARCH("Documentação",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Banco de dados">
+      <formula>NOT(ISERROR(SEARCH("Banco de dados",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Teste/análise">
+      <formula>NOT(ISERROR(SEARCH("Teste/análise",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
msgs para os adms e ajustes
</commit_message>
<xml_diff>
--- a/Arquivos/cronograma_tcc.xlsx
+++ b/Arquivos/cronograma_tcc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\TCC\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E2AFB2-0183-4FC2-85B7-713792DDB8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC6EB7C-CE89-4EE1-916B-DD89B8B1836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BBDFA246-CB9F-4529-AFA9-E3C590C6F618}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="85">
   <si>
     <t>Designer</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Folha de rosto</t>
+  </si>
+  <si>
+    <t>Capa</t>
+  </si>
+  <si>
+    <t>Dados de instalação</t>
   </si>
 </sst>
 </file>
@@ -682,22 +688,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -705,112 +711,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6699FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6699FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -872,82 +773,37 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="3" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFCCFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFCC99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -961,620 +817,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFCC99"/>
+          <bgColor rgb="FF6699FF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2062,7 +1312,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2070,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351F5228-FEA6-410A-9456-2C6350ABE72B}">
-  <dimension ref="C2:P64"/>
+  <dimension ref="C2:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,10 +1359,10 @@
       <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="41"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2124,7 +1374,7 @@
       </c>
     </row>
     <row r="3" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -2154,7 +1404,7 @@
       <c r="L3" s="37"/>
     </row>
     <row r="4" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="29" t="s">
@@ -2184,7 +1434,7 @@
       <c r="L4" s="36"/>
     </row>
     <row r="5" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="42" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -2214,7 +1464,7 @@
       <c r="L5" s="38"/>
     </row>
     <row r="6" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="29" t="s">
@@ -2244,7 +1494,7 @@
       <c r="L6" s="36"/>
     </row>
     <row r="7" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="42" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="27" t="s">
@@ -2274,7 +1524,7 @@
       <c r="L7" s="38"/>
     </row>
     <row r="8" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -2304,7 +1554,7 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="27" t="s">
@@ -2334,7 +1584,7 @@
       <c r="L9" s="38"/>
     </row>
     <row r="10" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="29" t="s">
@@ -2364,7 +1614,7 @@
       <c r="L10" s="36"/>
     </row>
     <row r="11" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="27" t="s">
@@ -2394,7 +1644,7 @@
       <c r="L11" s="38"/>
     </row>
     <row r="12" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="29" t="s">
@@ -2424,7 +1674,7 @@
       <c r="L12" s="36"/>
     </row>
     <row r="13" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="42" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -2454,7 +1704,7 @@
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="41" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="29" t="s">
@@ -2484,7 +1734,7 @@
       <c r="L14" s="36"/>
     </row>
     <row r="15" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="42" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="27" t="s">
@@ -2514,7 +1764,7 @@
       <c r="L15" s="38"/>
     </row>
     <row r="16" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -2544,7 +1794,7 @@
       <c r="L16" s="36"/>
     </row>
     <row r="17" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="27" t="s">
@@ -2574,7 +1824,7 @@
       <c r="L17" s="38"/>
     </row>
     <row r="18" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="29" t="s">
@@ -2604,7 +1854,7 @@
       <c r="L18" s="36"/>
     </row>
     <row r="19" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="42" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="27" t="s">
@@ -2634,7 +1884,7 @@
       <c r="L19" s="38"/>
     </row>
     <row r="20" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="41" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="29" t="s">
@@ -2664,7 +1914,7 @@
       <c r="L20" s="36"/>
     </row>
     <row r="21" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="42" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="27" t="s">
@@ -2694,7 +1944,7 @@
       <c r="L21" s="38"/>
     </row>
     <row r="22" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="29" t="s">
@@ -2725,7 +1975,7 @@
       <c r="P22" s="10"/>
     </row>
     <row r="23" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="27" t="s">
@@ -2756,7 +2006,7 @@
       <c r="P23" s="10"/>
     </row>
     <row r="24" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="41" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="29" t="s">
@@ -2787,7 +2037,7 @@
       <c r="P24" s="10"/>
     </row>
     <row r="25" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="27" t="s">
@@ -2818,7 +2068,7 @@
       <c r="P25" s="10"/>
     </row>
     <row r="26" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="29" t="s">
@@ -2849,7 +2099,7 @@
       <c r="P26" s="10"/>
     </row>
     <row r="27" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="42" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="27" t="s">
@@ -2880,7 +2130,7 @@
       <c r="P27" s="10"/>
     </row>
     <row r="28" spans="3:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="29" t="s">
@@ -2911,7 +2161,7 @@
       <c r="P28" s="10"/>
     </row>
     <row r="29" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="27" t="s">
@@ -2941,7 +2191,7 @@
       <c r="L29" s="38"/>
     </row>
     <row r="30" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="29" t="s">
@@ -2973,7 +2223,7 @@
       </c>
     </row>
     <row r="31" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="27" t="s">
@@ -3003,7 +2253,7 @@
       <c r="L31" s="38"/>
     </row>
     <row r="32" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="29" t="s">
@@ -3033,7 +2283,7 @@
       <c r="L32" s="36"/>
     </row>
     <row r="33" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="42" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="27" t="s">
@@ -3063,7 +2313,7 @@
       <c r="L33" s="38"/>
     </row>
     <row r="34" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="41" t="s">
         <v>30</v>
       </c>
       <c r="D34" s="29" t="s">
@@ -3093,7 +2343,7 @@
       <c r="L34" s="36"/>
     </row>
     <row r="35" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="27" t="s">
@@ -3123,7 +2373,7 @@
       <c r="L35" s="38"/>
     </row>
     <row r="36" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="29" t="s">
@@ -3155,7 +2405,7 @@
       </c>
     </row>
     <row r="37" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D37" s="27" t="s">
@@ -3185,7 +2435,7 @@
       <c r="L37" s="38"/>
     </row>
     <row r="38" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="41" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="29" t="s">
@@ -3215,7 +2465,7 @@
       <c r="L38" s="36"/>
     </row>
     <row r="39" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="27" t="s">
@@ -3245,7 +2495,7 @@
       <c r="L39" s="38"/>
     </row>
     <row r="40" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="29" t="s">
@@ -3277,7 +2527,7 @@
       </c>
     </row>
     <row r="41" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D41" s="27" t="s">
@@ -3307,7 +2557,7 @@
       <c r="L41" s="38"/>
     </row>
     <row r="42" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="29" t="s">
@@ -3337,7 +2587,7 @@
       <c r="L42" s="36"/>
     </row>
     <row r="43" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="27" t="s">
@@ -3367,7 +2617,7 @@
       <c r="L43" s="38"/>
     </row>
     <row r="44" spans="3:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="41" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="29" t="s">
@@ -3399,7 +2649,7 @@
       </c>
     </row>
     <row r="45" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="27" t="s">
@@ -3429,7 +2679,7 @@
       <c r="L45" s="38"/>
     </row>
     <row r="46" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C46" s="43" t="s">
+      <c r="C46" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="29" t="s">
@@ -3459,7 +2709,7 @@
       <c r="L46" s="36"/>
     </row>
     <row r="47" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="44" t="s">
+      <c r="C47" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D47" s="27" t="s">
@@ -3489,20 +2739,20 @@
       <c r="L47" s="38"/>
     </row>
     <row r="48" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E48" s="12">
         <v>45439</v>
       </c>
       <c r="F48" s="12">
-        <v>45440</v>
+        <v>45439</v>
       </c>
       <c r="G48" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>26</v>
@@ -3519,47 +2769,47 @@
       <c r="L48" s="36"/>
     </row>
     <row r="49" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C49" s="44" t="s">
-        <v>1</v>
+      <c r="C49" s="41" t="s">
+        <v>5</v>
       </c>
       <c r="D49" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="13">
+        <v>45439</v>
+      </c>
+      <c r="F49" s="13">
+        <v>45440</v>
+      </c>
+      <c r="G49" s="4">
+        <v>3</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K49" s="15">
+        <v>1</v>
+      </c>
+      <c r="L49" s="38"/>
+    </row>
+    <row r="50" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C50" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E50" s="12">
         <v>45446</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F50" s="12">
         <v>45448</v>
-      </c>
-      <c r="G49" s="4">
-        <v>4</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K49" s="15">
-        <v>0</v>
-      </c>
-      <c r="L49" s="38"/>
-    </row>
-    <row r="50" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C50" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="12">
-        <v>45451</v>
-      </c>
-      <c r="F50" s="12">
-        <v>45452</v>
       </c>
       <c r="G50" s="3">
         <v>4</v>
@@ -3579,20 +2829,20 @@
       <c r="L50" s="36"/>
     </row>
     <row r="51" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C51" s="44" t="s">
+      <c r="C51" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E51" s="13">
-        <v>45454</v>
+        <v>45451</v>
       </c>
       <c r="F51" s="13">
-        <v>45455</v>
+        <v>45452</v>
       </c>
       <c r="G51" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>26</v>
@@ -3609,20 +2859,20 @@
       <c r="L51" s="38"/>
     </row>
     <row r="52" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C52" s="43" t="s">
+      <c r="C52" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E52" s="12">
-        <v>45458</v>
+        <v>45454</v>
       </c>
       <c r="F52" s="12">
-        <v>45459</v>
+        <v>45455</v>
       </c>
       <c r="G52" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>26</v>
@@ -3639,20 +2889,20 @@
       <c r="L52" s="36"/>
     </row>
     <row r="53" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C53" s="44" t="s">
+      <c r="C53" s="41" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="13">
-        <v>45467</v>
+        <v>45458</v>
       </c>
       <c r="F53" s="13">
-        <v>45469</v>
+        <v>45459</v>
       </c>
       <c r="G53" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>26</v>
@@ -3669,20 +2919,20 @@
       <c r="L53" s="38"/>
     </row>
     <row r="54" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="42" t="s">
         <v>1</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E54" s="12">
-        <v>45471</v>
+        <v>45467</v>
       </c>
       <c r="F54" s="12">
-        <v>45472</v>
+        <v>45469</v>
       </c>
       <c r="G54" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>26</v>
@@ -3699,17 +2949,17 @@
       <c r="L54" s="36"/>
     </row>
     <row r="55" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C55" s="44" t="s">
-        <v>5</v>
+      <c r="C55" s="41" t="s">
+        <v>1</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E55" s="13">
-        <v>45443</v>
+        <v>45471</v>
       </c>
       <c r="F55" s="13">
-        <v>45443</v>
+        <v>45472</v>
       </c>
       <c r="G55" s="4">
         <v>3</v>
@@ -3718,7 +2968,7 @@
         <v>26</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="J55" s="7" t="s">
         <v>21</v>
@@ -3729,17 +2979,17 @@
       <c r="L55" s="38"/>
     </row>
     <row r="56" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C56" s="43" t="s">
+      <c r="C56" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E56" s="12">
-        <v>45450</v>
+        <v>45524</v>
       </c>
       <c r="F56" s="12">
-        <v>45450</v>
+        <v>45529</v>
       </c>
       <c r="G56" s="3">
         <v>2</v>
@@ -3751,25 +3001,25 @@
         <v>6</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K56" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L56" s="36"/>
     </row>
     <row r="57" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C57" s="44" t="s">
+      <c r="C57" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E57" s="13">
-        <v>45453</v>
+        <v>45529</v>
       </c>
       <c r="F57" s="13">
-        <v>45453</v>
+        <v>45531</v>
       </c>
       <c r="G57" s="4">
         <v>3</v>
@@ -3789,17 +3039,17 @@
       <c r="L57" s="38"/>
     </row>
     <row r="58" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C58" s="43" t="s">
+      <c r="C58" s="41" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E58" s="12">
-        <v>45457</v>
+        <v>45532</v>
       </c>
       <c r="F58" s="12">
-        <v>45457</v>
+        <v>45534</v>
       </c>
       <c r="G58" s="3">
         <v>2</v>
@@ -3819,20 +3069,20 @@
       <c r="L58" s="36"/>
     </row>
     <row r="59" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C59" s="44" t="s">
+      <c r="C59" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E59" s="13">
-        <v>45460</v>
+        <v>45535</v>
       </c>
       <c r="F59" s="13">
-        <v>45460</v>
+        <v>45537</v>
       </c>
       <c r="G59" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>26</v>
@@ -3849,47 +3099,107 @@
       <c r="L59" s="38"/>
     </row>
     <row r="60" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C60" s="45" t="s">
+      <c r="C60" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="12">
+        <v>45535</v>
+      </c>
+      <c r="F60" s="12">
+        <v>45537</v>
+      </c>
+      <c r="G60" s="3">
+        <v>2</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" s="15">
+        <v>0</v>
+      </c>
+      <c r="L60" s="36"/>
+    </row>
+    <row r="61" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C61" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61" s="13">
+        <v>45538</v>
+      </c>
+      <c r="F61" s="13">
+        <v>45541</v>
+      </c>
+      <c r="G61" s="4">
+        <v>4</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="15">
+        <v>0</v>
+      </c>
+      <c r="L61" s="38"/>
+    </row>
+    <row r="62" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C62" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E60" s="32">
+      <c r="E62" s="32">
         <v>45575</v>
       </c>
-      <c r="F60" s="32">
+      <c r="F62" s="32">
         <v>45585</v>
       </c>
-      <c r="G60" s="30">
+      <c r="G62" s="30">
         <v>4</v>
       </c>
-      <c r="H60" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I60" s="33" t="s">
+      <c r="H62" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="I62" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="J60" s="30" t="s">
+      <c r="J62" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="K60" s="34">
+      <c r="K62" s="34">
         <v>0</v>
       </c>
-      <c r="L60" s="39"/>
-    </row>
-    <row r="62" spans="3:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="C62" s="35" t="s">
+      <c r="L62" s="39"/>
+    </row>
+    <row r="64" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="C64" s="35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C63" s="35" t="s">
+    <row r="65" spans="3:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" s="35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="35" t="s">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="35" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3899,54 +3209,54 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A12:A15">
-    <cfRule type="duplicateValues" dxfId="28" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J60">
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Finalizado">
+  <conditionalFormatting sqref="C3:C62">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Teste/análise">
+      <formula>NOT(ISERROR(SEARCH("Teste/análise",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="Banco de dados">
+      <formula>NOT(ISERROR(SEARCH("Banco de dados",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Documentação">
+      <formula>NOT(ISERROR(SEARCH("Documentação",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Conteúdo">
+      <formula>NOT(ISERROR(SEARCH("Conteúdo",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Planejamento">
+      <formula>NOT(ISERROR(SEARCH("Planejamento",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Design">
+      <formula>NOT(ISERROR(SEARCH("Design",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Back-End">
+      <formula>NOT(ISERROR(SEARCH("Back-End",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Front-End">
+      <formula>NOT(ISERROR(SEARCH("Front-End",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J62">
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Finalizado">
       <formula>NOT(ISERROR(SEARCH("Finalizado",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="13" operator="containsText" text="A fazer">
+    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="A fazer">
       <formula>NOT(ISERROR(SEARCH("A fazer",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="Em progresso">
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="Em progresso">
       <formula>NOT(ISERROR(SEARCH("Em progresso",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K60">
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+  <conditionalFormatting sqref="K3:K62">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="greaterThan">
       <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C60">
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="Front-End">
-      <formula>NOT(ISERROR(SEARCH("Front-End",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="Back-End">
-      <formula>NOT(ISERROR(SEARCH("Back-End",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Design">
-      <formula>NOT(ISERROR(SEARCH("Design",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Planejamento">
-      <formula>NOT(ISERROR(SEARCH("Planejamento",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Conteúdo">
-      <formula>NOT(ISERROR(SEARCH("Conteúdo",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Documentação">
-      <formula>NOT(ISERROR(SEARCH("Documentação",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Banco de dados">
-      <formula>NOT(ISERROR(SEARCH("Banco de dados",C3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Teste/análise">
-      <formula>NOT(ISERROR(SEARCH("Teste/análise",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3958,19 +3268,19 @@
           <x14:formula1>
             <xm:f>Funções!$I$3:$I$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J60</xm:sqref>
+          <xm:sqref>J3:J62</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{04CB2B25-108D-4B1F-B63B-D01920EA7676}">
           <x14:formula1>
             <xm:f>Funções!$E$3:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C60</xm:sqref>
+          <xm:sqref>C3:C62</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9CC79E5-1BEA-4D87-92EF-20E7BD59CFBC}">
           <x14:formula1>
             <xm:f>Funções!$G$3:$G$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:I60</xm:sqref>
+          <xm:sqref>H3:I62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
css animais, att cron e ajustes gerais
</commit_message>
<xml_diff>
--- a/Arquivos/cronograma_tcc.xlsx
+++ b/Arquivos/cronograma_tcc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\TCC\Arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TCC-main\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC6EB7C-CE89-4EE1-916B-DD89B8B1836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C623CD6-CB79-4D66-9F83-5813E79697C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BBDFA246-CB9F-4529-AFA9-E3C590C6F618}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Cronograma" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cronograma!$C$2:$P$62</definedName>
     <definedName name="Sol1Dias" localSheetId="1">OFFSET(Cronograma!XFB1048576,MATCH(Cronograma!$M$19,Cronograma!XFC1:XFC14,0),,COUNTIF(Cronograma!XFC1:XFC14,Cronograma!$M$19))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -24,23 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="92">
   <si>
     <t>Designer</t>
   </si>
@@ -295,6 +285,27 @@
   </si>
   <si>
     <t>Dados de instalação</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>acordado em ststus do dia 26-8 a alteração da data final de abril para 30-9</t>
+  </si>
+  <si>
+    <t>próxima segunda</t>
+  </si>
+  <si>
+    <t>Manual - Operação/Uso</t>
+  </si>
+  <si>
+    <t>Manual - Manutenção</t>
+  </si>
+  <si>
+    <t>CSS - Footer</t>
+  </si>
+  <si>
+    <t>CSS - Mensagens</t>
   </si>
 </sst>
 </file>
@@ -589,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,6 +715,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -870,9 +884,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -910,7 +924,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1016,7 +1030,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1158,7 +1172,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1172,16 +1186,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="18" t="s">
         <v>22</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1267,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="20" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1297,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="22" t="s">
         <v>5</v>
       </c>
@@ -1295,17 +1309,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E9" s="24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E10" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="E11" s="25" t="s">
         <v>30</v>
       </c>
@@ -1320,30 +1334,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351F5228-FEA6-410A-9456-2C6350ABE72B}">
-  <dimension ref="C2:P66"/>
+  <dimension ref="C2:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="C48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" customWidth="1"/>
+    <col min="5" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="11" width="12.7265625" customWidth="1"/>
+    <col min="12" max="12" width="29.7265625" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" customWidth="1"/>
+    <col min="15" max="15" width="31.1796875" customWidth="1"/>
+    <col min="16" max="16" width="19.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1372,8 +1386,11 @@
       <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="M2" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C3" s="40" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +1420,7 @@
       </c>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C4" s="41" t="s">
         <v>10</v>
       </c>
@@ -1433,7 +1450,7 @@
       </c>
       <c r="L4" s="36"/>
     </row>
-    <row r="5" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="42" t="s">
         <v>11</v>
       </c>
@@ -1463,7 +1480,7 @@
       </c>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C6" s="41" t="s">
         <v>3</v>
       </c>
@@ -1493,7 +1510,7 @@
       </c>
       <c r="L6" s="36"/>
     </row>
-    <row r="7" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C7" s="42" t="s">
         <v>30</v>
       </c>
@@ -1523,7 +1540,7 @@
       </c>
       <c r="L7" s="38"/>
     </row>
-    <row r="8" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C8" s="41" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1570,7 @@
       </c>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C9" s="42" t="s">
         <v>11</v>
       </c>
@@ -1583,7 +1600,7 @@
       </c>
       <c r="L9" s="38"/>
     </row>
-    <row r="10" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C10" s="41" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1630,7 @@
       </c>
       <c r="L10" s="36"/>
     </row>
-    <row r="11" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C11" s="42" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1660,7 @@
       </c>
       <c r="L11" s="38"/>
     </row>
-    <row r="12" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C12" s="41" t="s">
         <v>5</v>
       </c>
@@ -1673,7 +1690,7 @@
       </c>
       <c r="L12" s="36"/>
     </row>
-    <row r="13" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C13" s="42" t="s">
         <v>30</v>
       </c>
@@ -1703,7 +1720,7 @@
       </c>
       <c r="L13" s="38"/>
     </row>
-    <row r="14" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C14" s="41" t="s">
         <v>31</v>
       </c>
@@ -1733,7 +1750,7 @@
       </c>
       <c r="L14" s="36"/>
     </row>
-    <row r="15" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C15" s="42" t="s">
         <v>11</v>
       </c>
@@ -1763,7 +1780,7 @@
       </c>
       <c r="L15" s="38"/>
     </row>
-    <row r="16" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C16" s="41" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1810,7 @@
       </c>
       <c r="L16" s="36"/>
     </row>
-    <row r="17" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C17" s="42" t="s">
         <v>1</v>
       </c>
@@ -1823,7 +1840,7 @@
       </c>
       <c r="L17" s="38"/>
     </row>
-    <row r="18" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C18" s="41" t="s">
         <v>5</v>
       </c>
@@ -1853,7 +1870,7 @@
       </c>
       <c r="L18" s="36"/>
     </row>
-    <row r="19" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C19" s="42" t="s">
         <v>30</v>
       </c>
@@ -1883,7 +1900,7 @@
       </c>
       <c r="L19" s="38"/>
     </row>
-    <row r="20" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C20" s="41" t="s">
         <v>31</v>
       </c>
@@ -1913,7 +1930,7 @@
       </c>
       <c r="L20" s="36"/>
     </row>
-    <row r="21" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C21" s="42" t="s">
         <v>11</v>
       </c>
@@ -1943,7 +1960,7 @@
       </c>
       <c r="L21" s="38"/>
     </row>
-    <row r="22" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C22" s="41" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +1991,7 @@
       <c r="L22" s="36"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C23" s="42" t="s">
         <v>1</v>
       </c>
@@ -2005,7 +2022,7 @@
       <c r="L23" s="38"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C24" s="41" t="s">
         <v>30</v>
       </c>
@@ -2036,7 +2053,7 @@
       <c r="L24" s="36"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C25" s="42" t="s">
         <v>31</v>
       </c>
@@ -2067,7 +2084,7 @@
       <c r="L25" s="38"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C26" s="41" t="s">
         <v>11</v>
       </c>
@@ -2098,7 +2115,7 @@
       <c r="L26" s="36"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C27" s="42" t="s">
         <v>3</v>
       </c>
@@ -2129,7 +2146,7 @@
       <c r="L27" s="38"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="3:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" ht="29" x14ac:dyDescent="0.35">
       <c r="C28" s="41" t="s">
         <v>1</v>
       </c>
@@ -2160,7 +2177,7 @@
       <c r="L28" s="36"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C29" s="42" t="s">
         <v>31</v>
       </c>
@@ -2190,7 +2207,7 @@
       </c>
       <c r="L29" s="38"/>
     </row>
-    <row r="30" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C30" s="41" t="s">
         <v>11</v>
       </c>
@@ -2201,7 +2218,7 @@
         <v>45411</v>
       </c>
       <c r="F30" s="12">
-        <v>45411</v>
+        <v>45565</v>
       </c>
       <c r="G30" s="3">
         <v>3</v>
@@ -2221,8 +2238,11 @@
       <c r="L30" s="36" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="M30" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C31" s="42" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2272,7 @@
       </c>
       <c r="L31" s="38"/>
     </row>
-    <row r="32" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:16" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C32" s="41" t="s">
         <v>1</v>
       </c>
@@ -2282,7 +2302,7 @@
       </c>
       <c r="L32" s="36"/>
     </row>
-    <row r="33" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C33" s="42" t="s">
         <v>3</v>
       </c>
@@ -2312,7 +2332,7 @@
       </c>
       <c r="L33" s="38"/>
     </row>
-    <row r="34" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C34" s="41" t="s">
         <v>30</v>
       </c>
@@ -2342,7 +2362,7 @@
       </c>
       <c r="L34" s="36"/>
     </row>
-    <row r="35" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C35" s="42" t="s">
         <v>31</v>
       </c>
@@ -2372,7 +2392,7 @@
       </c>
       <c r="L35" s="38"/>
     </row>
-    <row r="36" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C36" s="41" t="s">
         <v>11</v>
       </c>
@@ -2404,9 +2424,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C37" s="42" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D37" s="27" t="s">
         <v>52</v>
@@ -2427,14 +2447,14 @@
         <v>27</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K37" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="38"/>
     </row>
-    <row r="38" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C38" s="41" t="s">
         <v>3</v>
       </c>
@@ -2464,7 +2484,7 @@
       </c>
       <c r="L38" s="36"/>
     </row>
-    <row r="39" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C39" s="42" t="s">
         <v>31</v>
       </c>
@@ -2494,7 +2514,7 @@
       </c>
       <c r="L39" s="38"/>
     </row>
-    <row r="40" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C40" s="41" t="s">
         <v>11</v>
       </c>
@@ -2526,7 +2546,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C41" s="42" t="s">
         <v>28</v>
       </c>
@@ -2556,7 +2576,7 @@
       </c>
       <c r="L41" s="38"/>
     </row>
-    <row r="42" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C42" s="41" t="s">
         <v>1</v>
       </c>
@@ -2586,7 +2606,7 @@
       </c>
       <c r="L42" s="36"/>
     </row>
-    <row r="43" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C43" s="42" t="s">
         <v>31</v>
       </c>
@@ -2616,7 +2636,7 @@
       </c>
       <c r="L43" s="38"/>
     </row>
-    <row r="44" spans="3:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C44" s="41" t="s">
         <v>11</v>
       </c>
@@ -2648,7 +2668,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C45" s="42" t="s">
         <v>28</v>
       </c>
@@ -2678,7 +2698,7 @@
       </c>
       <c r="L45" s="38"/>
     </row>
-    <row r="46" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C46" s="41" t="s">
         <v>1</v>
       </c>
@@ -2708,7 +2728,7 @@
       </c>
       <c r="L46" s="36"/>
     </row>
-    <row r="47" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C47" s="42" t="s">
         <v>31</v>
       </c>
@@ -2738,7 +2758,7 @@
       </c>
       <c r="L47" s="38"/>
     </row>
-    <row r="48" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C48" s="42" t="s">
         <v>5</v>
       </c>
@@ -2768,7 +2788,7 @@
       </c>
       <c r="L48" s="36"/>
     </row>
-    <row r="49" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C49" s="41" t="s">
         <v>5</v>
       </c>
@@ -2798,7 +2818,7 @@
       </c>
       <c r="L49" s="38"/>
     </row>
-    <row r="50" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C50" s="42" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2848,7 @@
       </c>
       <c r="L50" s="36"/>
     </row>
-    <row r="51" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C51" s="41" t="s">
         <v>1</v>
       </c>
@@ -2858,7 +2878,7 @@
       </c>
       <c r="L51" s="38"/>
     </row>
-    <row r="52" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C52" s="42" t="s">
         <v>1</v>
       </c>
@@ -2888,7 +2908,7 @@
       </c>
       <c r="L52" s="36"/>
     </row>
-    <row r="53" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C53" s="41" t="s">
         <v>1</v>
       </c>
@@ -2918,7 +2938,7 @@
       </c>
       <c r="L53" s="38"/>
     </row>
-    <row r="54" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C54" s="42" t="s">
         <v>1</v>
       </c>
@@ -2948,7 +2968,7 @@
       </c>
       <c r="L54" s="36"/>
     </row>
-    <row r="55" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C55" s="41" t="s">
         <v>1</v>
       </c>
@@ -2971,14 +2991,14 @@
         <v>27</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K55" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55" s="38"/>
     </row>
-    <row r="56" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C56" s="41" t="s">
         <v>5</v>
       </c>
@@ -3001,14 +3021,14 @@
         <v>6</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K56" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L56" s="36"/>
     </row>
-    <row r="57" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C57" s="42" t="s">
         <v>5</v>
       </c>
@@ -3038,7 +3058,7 @@
       </c>
       <c r="L57" s="38"/>
     </row>
-    <row r="58" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C58" s="41" t="s">
         <v>5</v>
       </c>
@@ -3068,7 +3088,7 @@
       </c>
       <c r="L58" s="36"/>
     </row>
-    <row r="59" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C59" s="42" t="s">
         <v>5</v>
       </c>
@@ -3098,7 +3118,7 @@
       </c>
       <c r="L59" s="38"/>
     </row>
-    <row r="60" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C60" s="41" t="s">
         <v>5</v>
       </c>
@@ -3128,7 +3148,7 @@
       </c>
       <c r="L60" s="36"/>
     </row>
-    <row r="61" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C61" s="42" t="s">
         <v>5</v>
       </c>
@@ -3158,7 +3178,7 @@
       </c>
       <c r="L61" s="38"/>
     </row>
-    <row r="62" spans="3:12" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:12" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C62" s="43" t="s">
         <v>5</v>
       </c>
@@ -3188,22 +3208,49 @@
       </c>
       <c r="L62" s="39"/>
     </row>
-    <row r="64" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C64" s="35" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="65" spans="3:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C65" s="35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" s="35" t="s">
         <v>75</v>
       </c>
+      <c r="D66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="C2:P62" xr:uid="{10AA71E1-8C21-4C1B-8D0A-452C80674F87}">
+    <filterColumn colId="5" showButton="0"/>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="H2:I2"/>
   </mergeCells>
@@ -3237,7 +3284,7 @@
       <formula>NOT(ISERROR(SEARCH("Front-End",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J62">
+  <conditionalFormatting sqref="J3:J62 M30">
     <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Finalizado">
       <formula>NOT(ISERROR(SEARCH("Finalizado",J3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
att cronograma e manual técnico
</commit_message>
<xml_diff>
--- a/Arquivos/cronograma_tcc.xlsx
+++ b/Arquivos/cronograma_tcc.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Cronograma" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Cronograma!$C$2:$P$62</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Sol1Dias" vbProcedure="false">OFFSET(Cronograma!XFB1048576,MATCH(Cronograma!$M$19,Cronograma!XFC1:XFC14,0),,COUNTIF(Cronograma!XFC1:XFC14,Cronograma!$M$19))</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="93">
   <si>
     <t xml:space="preserve">Função</t>
   </si>
@@ -123,9 +122,6 @@
     <t xml:space="preserve">Observação</t>
   </si>
   <si>
-    <t xml:space="preserve">obs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Geral (tarefas, funções e cronograma definidos)</t>
   </si>
   <si>
@@ -265,6 +261,18 @@
   </si>
   <si>
     <t xml:space="preserve">Lista de materiais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Página Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação sobre o que é o projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSS – Ajustes finais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrigir erros e/ou pequenos detalhes que deixamos passar</t>
   </si>
   <si>
     <t xml:space="preserve">Suporte</t>
@@ -499,13 +507,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -521,6 +522,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="thin"/>
       <top/>
       <bottom/>
@@ -581,196 +589,204 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="13" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="15" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="14" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="12" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,7 +799,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -909,14 +925,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FF006100"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
@@ -926,21 +934,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF9C0006"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9C5700"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1135,10 +1128,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office 2013 - 2022">
   <a:themeElements>
@@ -1318,145 +1307,145 @@
   </sheetPr>
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C3" s="6" t="str">
         <f aca="false">G4&amp;G5</f>
         <v>Isabela Adryelly </v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C4" s="6" t="str">
         <f aca="false">G5&amp;G6</f>
         <v>Adryelly Gabriel </v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="C5" s="6" t="str">
         <f aca="false">G5&amp;G6</f>
         <v>Adryelly Gabriel </v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="str">
+      <c r="C6" s="6" t="str">
         <f aca="false">G5&amp;G6</f>
         <v>Adryelly Gabriel </v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="str">
+      <c r="C7" s="6" t="str">
         <f aca="false">G4&amp;G7</f>
         <v>Isabela Pablo </v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9" t="str">
+      <c r="C8" s="10" t="str">
         <f aca="false">G5&amp;G7</f>
         <v>Adryelly Pablo </v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1476,71 +1465,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C2:P68"/>
+  <dimension ref="C2:P70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I24" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L60" activeCellId="0" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="M2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="16" t="n">
         <v>45376</v>
@@ -1570,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="24" t="n">
         <v>45380</v>
@@ -1600,7 +1587,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="31" t="n">
         <v>45385</v>
@@ -1630,7 +1617,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="24" t="n">
         <v>45383</v>
@@ -1660,7 +1647,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="31" t="n">
         <v>45383</v>
@@ -1690,7 +1677,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="24" t="n">
         <v>45386</v>
@@ -1720,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="31" t="n">
         <v>45387</v>
@@ -1750,7 +1737,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="24" t="n">
         <v>45384</v>
@@ -1780,7 +1767,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="31" t="n">
         <v>45386</v>
@@ -1810,7 +1797,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="24" t="n">
         <v>45390</v>
@@ -1840,7 +1827,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="31" t="n">
         <v>45392</v>
@@ -1870,7 +1857,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="24" t="n">
         <v>45394</v>
@@ -1900,7 +1887,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="31" t="n">
         <v>45396</v>
@@ -1930,7 +1917,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="24" t="n">
         <v>45397</v>
@@ -1960,7 +1947,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="31" t="n">
         <v>45398</v>
@@ -1990,7 +1977,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="24" t="n">
         <v>45400</v>
@@ -2020,7 +2007,7 @@
         <v>24</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="31" t="n">
         <v>45401</v>
@@ -2050,7 +2037,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="24" t="n">
         <v>45402</v>
@@ -2080,7 +2067,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="31" t="n">
         <v>45403</v>
@@ -2110,7 +2097,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="24" t="n">
         <v>45404</v>
@@ -2141,7 +2128,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="31" t="n">
         <v>45405</v>
@@ -2172,7 +2159,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="24" t="n">
         <v>45404</v>
@@ -2203,7 +2190,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="31" t="n">
         <v>45407</v>
@@ -2234,7 +2221,7 @@
         <v>14</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="24" t="n">
         <v>45408</v>
@@ -2265,7 +2252,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="31" t="n">
         <v>45409</v>
@@ -2296,7 +2283,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="24" t="n">
         <v>45410</v>
@@ -2327,7 +2314,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="31" t="n">
         <v>45411</v>
@@ -2357,7 +2344,7 @@
         <v>14</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="24" t="n">
         <v>45565</v>
@@ -2381,7 +2368,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M30" s="38"/>
     </row>
@@ -2390,7 +2377,7 @@
         <v>20</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="31" t="n">
         <v>45412</v>
@@ -2420,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="24" t="n">
         <v>45414</v>
@@ -2450,7 +2437,7 @@
         <v>17</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="31" t="n">
         <v>45415</v>
@@ -2480,7 +2467,7 @@
         <v>24</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" s="24" t="n">
         <v>45568</v>
@@ -2510,7 +2497,7 @@
         <v>23</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E35" s="31" t="n">
         <v>45417</v>
@@ -2540,7 +2527,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="24" t="n">
         <v>45572</v>
@@ -2564,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="L36" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2572,7 +2559,7 @@
         <v>24</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E37" s="31" t="n">
         <v>45419</v>
@@ -2602,7 +2589,7 @@
         <v>17</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" s="24" t="n">
         <v>45422</v>
@@ -2632,7 +2619,7 @@
         <v>23</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="31" t="n">
         <v>45423</v>
@@ -2662,7 +2649,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40" s="24" t="n">
         <v>45575</v>
@@ -2686,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,7 +2681,7 @@
         <v>20</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" s="31" t="n">
         <v>45427</v>
@@ -2724,7 +2711,7 @@
         <v>9</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" s="24" t="n">
         <v>45430</v>
@@ -2754,7 +2741,7 @@
         <v>23</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E43" s="31" t="n">
         <v>45432</v>
@@ -2784,7 +2771,7 @@
         <v>14</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" s="24" t="n">
         <v>45579</v>
@@ -2808,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,7 +2803,7 @@
         <v>20</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45" s="31" t="n">
         <v>45439</v>
@@ -2846,7 +2833,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46" s="24" t="n">
         <v>45442</v>
@@ -2864,10 +2851,10 @@
         <v>18</v>
       </c>
       <c r="J46" s="26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K46" s="36" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L46" s="28"/>
     </row>
@@ -2876,7 +2863,7 @@
         <v>23</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E47" s="31" t="n">
         <v>45439</v>
@@ -2906,7 +2893,7 @@
         <v>22</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" s="24" t="n">
         <v>45439</v>
@@ -2936,7 +2923,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" s="31" t="n">
         <v>45439</v>
@@ -2966,7 +2953,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E50" s="24" t="n">
         <v>45446</v>
@@ -2996,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E51" s="31" t="n">
         <v>45451</v>
@@ -3014,10 +3001,10 @@
         <v>18</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K51" s="36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="35"/>
     </row>
@@ -3026,7 +3013,7 @@
         <v>9</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E52" s="24" t="n">
         <v>45454</v>
@@ -3056,7 +3043,7 @@
         <v>9</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" s="31" t="n">
         <v>45458</v>
@@ -3074,10 +3061,10 @@
         <v>18</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K53" s="36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" s="35"/>
     </row>
@@ -3086,7 +3073,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E54" s="24" t="n">
         <v>45467</v>
@@ -3104,10 +3091,10 @@
         <v>18</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K54" s="36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="28"/>
     </row>
@@ -3116,7 +3103,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E55" s="31" t="n">
         <v>45471</v>
@@ -3146,7 +3133,7 @@
         <v>22</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E56" s="24" t="n">
         <v>45524</v>
@@ -3176,7 +3163,7 @@
         <v>22</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E57" s="31" t="n">
         <v>45529</v>
@@ -3206,7 +3193,7 @@
         <v>22</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E58" s="24" t="n">
         <v>45532</v>
@@ -3236,7 +3223,7 @@
         <v>22</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" s="31" t="n">
         <v>45535</v>
@@ -3261,57 +3248,59 @@
       </c>
       <c r="L59" s="35"/>
     </row>
-    <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E60" s="24" t="n">
-        <v>45535</v>
+        <v>45520</v>
       </c>
       <c r="F60" s="24" t="n">
-        <v>45537</v>
+        <v>45565</v>
       </c>
       <c r="G60" s="25" t="n">
         <v>2</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I60" s="26" t="s">
         <v>21</v>
       </c>
       <c r="J60" s="26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K60" s="36" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L60" s="28"/>
-    </row>
-    <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="L60" s="39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="29" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D61" s="30" t="s">
         <v>81</v>
       </c>
       <c r="E61" s="31" t="n">
-        <v>45538</v>
+        <v>45551</v>
       </c>
       <c r="F61" s="31" t="n">
         <v>45565</v>
       </c>
       <c r="G61" s="32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H61" s="33" t="s">
         <v>15</v>
       </c>
       <c r="I61" s="33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J61" s="26" t="s">
         <v>8</v>
@@ -3319,151 +3308,210 @@
       <c r="K61" s="36" t="n">
         <v>0</v>
       </c>
-      <c r="L61" s="35"/>
+      <c r="L61" s="40" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="39" t="s">
+      <c r="C62" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="E62" s="41" t="n">
+      <c r="D62" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E62" s="24" t="n">
+        <v>45535</v>
+      </c>
+      <c r="F62" s="24" t="n">
+        <v>45537</v>
+      </c>
+      <c r="G62" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="H62" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" s="28"/>
+    </row>
+    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" s="31" t="n">
+        <v>45538</v>
+      </c>
+      <c r="F63" s="31" t="n">
+        <v>45565</v>
+      </c>
+      <c r="G63" s="32" t="n">
+        <v>4</v>
+      </c>
+      <c r="H63" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J63" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K63" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" s="35"/>
+    </row>
+    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="43" t="n">
         <v>45575</v>
       </c>
-      <c r="F62" s="41" t="n">
+      <c r="F64" s="43" t="n">
         <v>45585</v>
       </c>
-      <c r="G62" s="42" t="n">
+      <c r="G64" s="44" t="n">
         <v>4</v>
       </c>
-      <c r="H62" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="I62" s="43" t="s">
+      <c r="H64" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="J62" s="44" t="s">
+      <c r="J64" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="K62" s="45" t="n">
+      <c r="K64" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="L62" s="46"/>
-    </row>
-    <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D65" s="0" t="s">
+      <c r="L64" s="48"/>
+    </row>
+    <row r="66" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="49" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="47" t="s">
+      <c r="D66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="0" t="s">
+    </row>
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="49" t="s">
         <v>88</v>
       </c>
+      <c r="D67" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="0" t="s">
-        <v>89</v>
+      <c r="C68" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D70" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:P62">
-    <filterColumn colId="0" hiddenButton="1"/>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="H2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C62">
-    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Teste/análise" dxfId="20">
+  <conditionalFormatting sqref="C3:C64">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Teste/análise" dxfId="17">
       <formula>NOT(ISERROR(SEARCH("Teste/análise",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Banco de dados" dxfId="21">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Banco de dados" dxfId="18">
       <formula>NOT(ISERROR(SEARCH("Banco de dados",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Documentação" dxfId="22">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Documentação" dxfId="19">
       <formula>NOT(ISERROR(SEARCH("Documentação",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Conteúdo" dxfId="23">
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Conteúdo" dxfId="20">
       <formula>NOT(ISERROR(SEARCH("Conteúdo",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Planejamento" dxfId="24">
+    <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Planejamento" dxfId="21">
       <formula>NOT(ISERROR(SEARCH("Planejamento",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Design" dxfId="25">
+    <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Design" dxfId="22">
       <formula>NOT(ISERROR(SEARCH("Design",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Back-End" dxfId="26">
+    <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Back-End" dxfId="23">
       <formula>NOT(ISERROR(SEARCH("Back-End",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Front-End" dxfId="27">
+    <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Front-End" dxfId="24">
       <formula>NOT(ISERROR(SEARCH("Front-End",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J62">
-    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Finalizado" dxfId="28">
+  <conditionalFormatting sqref="J3:J64">
+    <cfRule type="containsText" priority="10" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Finalizado" dxfId="25">
       <formula>NOT(ISERROR(SEARCH("Finalizado",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="A fazer" dxfId="29">
+    <cfRule type="containsText" priority="11" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="A fazer" dxfId="26">
       <formula>NOT(ISERROR(SEARCH("A fazer",J3)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Em progresso" dxfId="30">
+    <cfRule type="containsText" priority="12" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Em progresso" dxfId="27">
       <formula>NOT(ISERROR(SEARCH("Em progresso",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K62">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+  <conditionalFormatting sqref="K3:K64">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="cellIs" priority="15" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A15">
-    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34"/>
+    <cfRule type="duplicateValues" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30">
-    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Finalizado" dxfId="28">
+    <cfRule type="containsText" priority="17" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Finalizado" dxfId="25">
       <formula>NOT(ISERROR(SEARCH("Finalizado",M30)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="A fazer" dxfId="29">
+    <cfRule type="containsText" priority="18" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="A fazer" dxfId="26">
       <formula>NOT(ISERROR(SEARCH("A fazer",M30)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Em progresso" dxfId="30">
+    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Em progresso" dxfId="27">
       <formula>NOT(ISERROR(SEARCH("Em progresso",M30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3:J62" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J3:J64" type="list">
       <formula1>Funções!$I$3:$I$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C62" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C64" type="list">
       <formula1>Funções!$E$3:$E$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:I62" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H3:I64" type="list">
       <formula1>Funções!$G$3:$G$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3475,6 +3523,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>